<commit_message>
Purchase entry UI changes
</commit_message>
<xml_diff>
--- a/src/main/java/com/pharmeasy/MercuryUI/Data/webTestData.xlsx
+++ b/src/main/java/com/pharmeasy/MercuryUI/Data/webTestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="SalesReturnBarcode" sheetId="1" r:id="rId1"/>
@@ -137,19 +137,19 @@
     <t>CROCIN ADVANCE 500MG TAB</t>
   </si>
   <si>
-    <t>XCEF 200MG TAB</t>
-  </si>
-  <si>
-    <t>new741</t>
-  </si>
-  <si>
-    <t>new742</t>
-  </si>
-  <si>
-    <t>new743</t>
-  </si>
-  <si>
     <t>Test</t>
+  </si>
+  <si>
+    <t>GOLD COAT LOTION 120ML</t>
+  </si>
+  <si>
+    <t>ne31</t>
+  </si>
+  <si>
+    <t>ne12</t>
+  </si>
+  <si>
+    <t>ne41</t>
   </si>
 </sst>
 </file>
@@ -668,8 +668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -694,7 +694,7 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -706,8 +706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -727,7 +727,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>31</v>
@@ -735,7 +735,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>32</v>
@@ -743,10 +743,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>